<commit_message>
completed Mini Project for submission
This is my first mini project submitted in partial fulfillment for the award of a certificate in Data Analytics at Cyclobold School of Software Engineering
</commit_message>
<xml_diff>
--- a/MINI PROJECT DAX SALES DASHBOARD.xlsx
+++ b/MINI PROJECT DAX SALES DASHBOARD.xlsx
@@ -4372,162 +4372,18 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>573380</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>141282</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>179654</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>70412</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="16" name="Product Name 2"/>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Product Name 2"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="1176630" y="1093782"/>
-              <a:ext cx="5035524" cy="691130"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
-If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>481584</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>15690</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>489742</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>7668</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="6" name="Customer"/>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
-              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Customer"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6514084" y="4587690"/>
-              <a:ext cx="6040658" cy="372978"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
-If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9320</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>52</xdr:col>
-      <xdr:colOff>174625</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>34018</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>8030</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -4536,10 +4392,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9320" y="0"/>
-          <a:ext cx="36280930" cy="17369518"/>
-          <a:chOff x="310945" y="76814"/>
-          <a:chExt cx="36280930" cy="17369518"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="22755971" cy="8873191"/>
+          <a:chOff x="-36691630" y="132733"/>
+          <a:chExt cx="157864776" cy="9054537"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -4549,8 +4405,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="310945" y="76814"/>
-            <a:ext cx="36280930" cy="17369518"/>
+            <a:off x="-36691630" y="132733"/>
+            <a:ext cx="157864776" cy="9054537"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -4622,8 +4478,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="798035" y="155907"/>
-            <a:ext cx="12918409" cy="729892"/>
+            <a:off x="-16732102" y="214453"/>
+            <a:ext cx="99498564" cy="729892"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
             <a:avLst/>
@@ -4684,8 +4540,8 @@
           <xdr:cNvGraphicFramePr/>
         </xdr:nvGraphicFramePr>
         <xdr:xfrm>
-          <a:off x="7544622" y="5186595"/>
-          <a:ext cx="3582729" cy="2097471"/>
+          <a:off x="6025096" y="6458178"/>
+          <a:ext cx="38610779" cy="2436000"/>
         </xdr:xfrm>
         <a:graphic>
           <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4699,8 +4555,8 @@
           <xdr:cNvGraphicFramePr/>
         </xdr:nvGraphicFramePr>
         <xdr:xfrm>
-          <a:off x="1036687" y="2136275"/>
-          <a:ext cx="5191533" cy="2686204"/>
+          <a:off x="-31638633" y="1905143"/>
+          <a:ext cx="56230824" cy="3258946"/>
         </xdr:xfrm>
         <a:graphic>
           <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4714,8 +4570,8 @@
           <xdr:cNvGraphicFramePr/>
         </xdr:nvGraphicFramePr>
         <xdr:xfrm>
-          <a:off x="7983225" y="1086135"/>
-          <a:ext cx="7139574" cy="3244637"/>
+          <a:off x="25499138" y="1934596"/>
+          <a:ext cx="72167202" cy="3248552"/>
         </xdr:xfrm>
         <a:graphic>
           <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4724,6 +4580,150 @@
         </a:graphic>
       </xdr:graphicFrame>
     </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>560293</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>110933</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>504264</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="16" name="Product Name 2"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Product Name 2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4258234" y="857992"/>
+              <a:ext cx="9805148" cy="748185"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>240462</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>139090</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>248618</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>131068</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="6" name="Customer"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Customer"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5787374" y="5555266"/>
+              <a:ext cx="6171391" cy="365508"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -8017,15 +8017,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="AG2:AI41"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AG30" sqref="AF30:AG32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="51" zoomScaleNormal="80" zoomScaleSheetLayoutView="51" workbookViewId="0">
+      <selection activeCell="Z32" sqref="Z32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="33" max="33" width="25.42578125" customWidth="1"/>
-    <col min="34" max="34" width="22.28515625" customWidth="1"/>
-    <col min="35" max="35" width="32.5703125" customWidth="1"/>
+    <col min="33" max="33" width="24.5703125" customWidth="1"/>
+    <col min="34" max="34" width="20.85546875" customWidth="1"/>
+    <col min="35" max="35" width="31.28515625" customWidth="1"/>
     <col min="36" max="36" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>